<commit_message>
- K opt data pt2
</commit_message>
<xml_diff>
--- a/src/output/opt/K/data.xlsx
+++ b/src/output/opt/K/data.xlsx
@@ -63,7 +63,7 @@
     <col min="2" max="2" width="5" customWidth="true"/>
     <col min="3" max="3" width="2" customWidth="true"/>
     <col min="4" max="4" width="3.5546875" customWidth="true"/>
-    <col min="5" max="5" width="4" customWidth="true"/>
+    <col min="5" max="5" width="5" customWidth="true"/>
     <col min="6" max="6" width="4" customWidth="true"/>
     <col min="7" max="7" width="4.5546875" customWidth="true"/>
     <col min="8" max="8" width="3" customWidth="true"/>
@@ -89,7 +89,7 @@
         <v>2.5</v>
       </c>
       <c r="E1" s="0">
-        <v>0.10000000000000001</v>
+        <v>200</v>
       </c>
       <c r="F1" s="0">
         <v>100</v>
@@ -104,13 +104,13 @@
         <v>209</v>
       </c>
       <c r="J1" s="0">
-        <v>11.802967000000001</v>
+        <v>11.469571800000001</v>
       </c>
       <c r="K1" s="0">
-        <v>6.4177040765667215e-05</v>
+        <v>5.6270252276391375e-05</v>
       </c>
       <c r="L1" s="0">
-        <v>7.1536401133504575e-07</v>
+        <v>3.5884963364348802e-07</v>
       </c>
       <c r="M1" s="0">
         <v>0</v>
@@ -133,7 +133,7 @@
         <v>2.5</v>
       </c>
       <c r="E2" s="0">
-        <v>0.10000000000000001</v>
+        <v>200</v>
       </c>
       <c r="F2" s="0">
         <v>100</v>
@@ -148,13 +148,13 @@
         <v>269</v>
       </c>
       <c r="J2" s="0">
-        <v>78.696667599999998</v>
+        <v>85.998538100000005</v>
       </c>
       <c r="K2" s="0">
-        <v>6.6339441054497073e-05</v>
+        <v>5.7291579179885588e-05</v>
       </c>
       <c r="L2" s="0">
-        <v>5.1314608821732135e-07</v>
+        <v>2.9056295748841403e-07</v>
       </c>
       <c r="M2" s="0">
         <v>0</v>
@@ -177,7 +177,7 @@
         <v>2.5</v>
       </c>
       <c r="E3" s="0">
-        <v>0.10000000000000001</v>
+        <v>200</v>
       </c>
       <c r="F3" s="0">
         <v>100</v>
@@ -189,22 +189,22 @@
         <v>10</v>
       </c>
       <c r="I3" s="0">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J3" s="0">
-        <v>83.839222800000002</v>
+        <v>87.064598700000005</v>
       </c>
       <c r="K3" s="0">
-        <v>0.0002330072599801003</v>
+        <v>0.00028043565219437738</v>
       </c>
       <c r="L3" s="0">
-        <v>-2.4749957986818785e-05</v>
+        <v>-1.2757075532769695e-05</v>
       </c>
       <c r="M3" s="0">
         <v>1</v>
       </c>
       <c r="N3" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4">
@@ -221,7 +221,7 @@
         <v>2.5</v>
       </c>
       <c r="E4" s="0">
-        <v>0.10000000000000001</v>
+        <v>200</v>
       </c>
       <c r="F4" s="0">
         <v>100</v>
@@ -233,22 +233,22 @@
         <v>10</v>
       </c>
       <c r="I4" s="0">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J4" s="0">
-        <v>179.43920220000001</v>
+        <v>213.07385719999999</v>
       </c>
       <c r="K4" s="0">
-        <v>0.00069614310459442663</v>
+        <v>0.00056235209555466348</v>
       </c>
       <c r="L4" s="0">
-        <v>-2.6525707986836933e-05</v>
+        <v>-4.4311236558517197e-05</v>
       </c>
       <c r="M4" s="0">
         <v>2</v>
       </c>
       <c r="N4" s="0">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5">
@@ -265,7 +265,7 @@
         <v>2.5</v>
       </c>
       <c r="E5" s="0">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="F5" s="0">
         <v>100</v>
@@ -280,13 +280,13 @@
         <v>209</v>
       </c>
       <c r="J5" s="0">
-        <v>10.6848478</v>
+        <v>11.617077200000001</v>
       </c>
       <c r="K5" s="0">
-        <v>6.3995185423992851e-05</v>
+        <v>4.4798810441504244e-05</v>
       </c>
       <c r="L5" s="0">
-        <v>7.2015366786396012e-07</v>
+        <v>2.2382705932867137e-07</v>
       </c>
       <c r="M5" s="0">
         <v>0</v>
@@ -309,7 +309,7 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="0">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="F6" s="0">
         <v>100</v>
@@ -324,13 +324,13 @@
         <v>269</v>
       </c>
       <c r="J6" s="0">
-        <v>115.7776236</v>
+        <v>123.7624783</v>
       </c>
       <c r="K6" s="0">
-        <v>6.5670124112848782e-05</v>
+        <v>5.2544187840064538e-05</v>
       </c>
       <c r="L6" s="0">
-        <v>5.0828665924781935e-07</v>
+        <v>1.2266450801404607e-07</v>
       </c>
       <c r="M6" s="0">
         <v>0</v>
@@ -353,7 +353,7 @@
         <v>2.5</v>
       </c>
       <c r="E7" s="0">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="F7" s="0">
         <v>100</v>
@@ -368,13 +368,13 @@
         <v>251</v>
       </c>
       <c r="J7" s="0">
-        <v>87.705304999999996</v>
+        <v>97.262322100000006</v>
       </c>
       <c r="K7" s="0">
-        <v>0.00017392714633945872</v>
+        <v>0.00030585836905561159</v>
       </c>
       <c r="L7" s="0">
-        <v>-2.3095603817279466e-05</v>
+        <v>-2.7164391021007578e-05</v>
       </c>
       <c r="M7" s="0">
         <v>1</v>
@@ -397,7 +397,7 @@
         <v>2.5</v>
       </c>
       <c r="E8" s="0">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="F8" s="0">
         <v>100</v>
@@ -412,19 +412,19 @@
         <v>271</v>
       </c>
       <c r="J8" s="0">
-        <v>214.46668869999999</v>
+        <v>194.27795739999999</v>
       </c>
       <c r="K8" s="0">
-        <v>0.00067322016645099403</v>
+        <v>0.00046422798192669035</v>
       </c>
       <c r="L8" s="0">
-        <v>-3.7358803296911815e-05</v>
+        <v>-3.819826392043179e-05</v>
       </c>
       <c r="M8" s="0">
         <v>2</v>
       </c>
       <c r="N8" s="0">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9">
@@ -441,7 +441,7 @@
         <v>2.5</v>
       </c>
       <c r="E9" s="0">
-        <v>5</v>
+        <v>600</v>
       </c>
       <c r="F9" s="0">
         <v>100</v>
@@ -456,13 +456,13 @@
         <v>209</v>
       </c>
       <c r="J9" s="0">
-        <v>10.276679</v>
+        <v>10.9386533</v>
       </c>
       <c r="K9" s="0">
-        <v>6.3846390175203993e-05</v>
+        <v>0.00030741117852550737</v>
       </c>
       <c r="L9" s="0">
-        <v>7.1189755656960133e-07</v>
+        <v>1.590219940428454e-06</v>
       </c>
       <c r="M9" s="0">
         <v>0</v>
@@ -485,7 +485,7 @@
         <v>2.5</v>
       </c>
       <c r="E10" s="0">
-        <v>5</v>
+        <v>600</v>
       </c>
       <c r="F10" s="0">
         <v>100</v>
@@ -497,16 +497,16 @@
         <v>10</v>
       </c>
       <c r="I10" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J10" s="0">
-        <v>96.294264600000005</v>
+        <v>92.545244400000001</v>
       </c>
       <c r="K10" s="0">
-        <v>6.6175797355239041e-05</v>
+        <v>5.2308786186339162e-05</v>
       </c>
       <c r="L10" s="0">
-        <v>5.142693354762604e-07</v>
+        <v>-1.8850709496624299e-06</v>
       </c>
       <c r="M10" s="0">
         <v>0</v>
@@ -529,7 +529,7 @@
         <v>2.5</v>
       </c>
       <c r="E11" s="0">
-        <v>5</v>
+        <v>600</v>
       </c>
       <c r="F11" s="0">
         <v>100</v>
@@ -544,13 +544,13 @@
         <v>251</v>
       </c>
       <c r="J11" s="0">
-        <v>90.141661200000001</v>
+        <v>91.648784699999993</v>
       </c>
       <c r="K11" s="0">
-        <v>0.00023388839137461481</v>
+        <v>0.00025894574966001116</v>
       </c>
       <c r="L11" s="0">
-        <v>-2.5168598372863147e-05</v>
+        <v>-1.9674145135171105e-05</v>
       </c>
       <c r="M11" s="0">
         <v>1</v>
@@ -573,7 +573,7 @@
         <v>2.5</v>
       </c>
       <c r="E12" s="0">
-        <v>5</v>
+        <v>600</v>
       </c>
       <c r="F12" s="0">
         <v>100</v>
@@ -585,22 +585,22 @@
         <v>10</v>
       </c>
       <c r="I12" s="0">
-        <v>269</v>
+        <v>493</v>
       </c>
       <c r="J12" s="0">
-        <v>197.63692900000001</v>
+        <v>465.7934128</v>
       </c>
       <c r="K12" s="0">
-        <v>0.00048299551221075987</v>
+        <v>0.0016784108346536986</v>
       </c>
       <c r="L12" s="0">
-        <v>-4.4883933796153063e-05</v>
+        <v>-0.0024044526872350658</v>
       </c>
       <c r="M12" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N12" s="0">
-        <v>172</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13">
@@ -617,7 +617,7 @@
         <v>2.5</v>
       </c>
       <c r="E13" s="0">
-        <v>10</v>
+        <v>800</v>
       </c>
       <c r="F13" s="0">
         <v>100</v>
@@ -632,13 +632,13 @@
         <v>209</v>
       </c>
       <c r="J13" s="0">
-        <v>10.199197699999999</v>
+        <v>11.8562732</v>
       </c>
       <c r="K13" s="0">
-        <v>6.3456254398186474e-05</v>
+        <v>0.00025028350163358581</v>
       </c>
       <c r="L13" s="0">
-        <v>7.0544782584561883e-07</v>
+        <v>1.2326467092179433e-06</v>
       </c>
       <c r="M13" s="0">
         <v>0</v>
@@ -661,7 +661,7 @@
         <v>2.5</v>
       </c>
       <c r="E14" s="0">
-        <v>10</v>
+        <v>800</v>
       </c>
       <c r="F14" s="0">
         <v>100</v>
@@ -673,22 +673,22 @@
         <v>10</v>
       </c>
       <c r="I14" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J14" s="0">
-        <v>107.1313579</v>
+        <v>113.974687</v>
       </c>
       <c r="K14" s="0">
-        <v>6.5997330021216882e-05</v>
+        <v>5.2793127088612835e-05</v>
       </c>
       <c r="L14" s="0">
-        <v>4.8492216979766602e-07</v>
+        <v>-1.4276651805418591e-06</v>
       </c>
       <c r="M14" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="0">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
@@ -705,7 +705,7 @@
         <v>2.5</v>
       </c>
       <c r="E15" s="0">
-        <v>10</v>
+        <v>800</v>
       </c>
       <c r="F15" s="0">
         <v>100</v>
@@ -717,22 +717,22 @@
         <v>10</v>
       </c>
       <c r="I15" s="0">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J15" s="0">
-        <v>88.606640999999996</v>
+        <v>92.5555181</v>
       </c>
       <c r="K15" s="0">
-        <v>0.00020161746254965252</v>
+        <v>0.00091414444702575537</v>
       </c>
       <c r="L15" s="0">
-        <v>-2.3781491897126006e-05</v>
+        <v>-9.1632819965110627e-06</v>
       </c>
       <c r="M15" s="0">
         <v>1</v>
       </c>
       <c r="N15" s="0">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -749,7 +749,7 @@
         <v>2.5</v>
       </c>
       <c r="E16" s="0">
-        <v>10</v>
+        <v>800</v>
       </c>
       <c r="F16" s="0">
         <v>100</v>
@@ -761,16 +761,16 @@
         <v>10</v>
       </c>
       <c r="I16" s="0">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J16" s="0">
-        <v>197.35563490000001</v>
+        <v>232.82780260000001</v>
       </c>
       <c r="K16" s="0">
-        <v>0.00078415626376182601</v>
+        <v>0.00050787581890743283</v>
       </c>
       <c r="L16" s="0">
-        <v>-3.0608607912803039e-05</v>
+        <v>-2.271357437524097e-05</v>
       </c>
       <c r="M16" s="0">
         <v>2</v>
@@ -793,7 +793,7 @@
         <v>2.5</v>
       </c>
       <c r="E17" s="0">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F17" s="0">
         <v>100</v>
@@ -808,13 +808,13 @@
         <v>209</v>
       </c>
       <c r="J17" s="0">
-        <v>11.457540099999999</v>
+        <v>13.0947622</v>
       </c>
       <c r="K17" s="0">
-        <v>5.6488426352085952e-05</v>
+        <v>0.00020984865798445718</v>
       </c>
       <c r="L17" s="0">
-        <v>5.2850555026397074e-07</v>
+        <v>6.8207856344959414e-07</v>
       </c>
       <c r="M17" s="0">
         <v>0</v>
@@ -837,7 +837,7 @@
         <v>2.5</v>
       </c>
       <c r="E18" s="0">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F18" s="0">
         <v>100</v>
@@ -849,22 +849,22 @@
         <v>10</v>
       </c>
       <c r="I18" s="0">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J18" s="0">
-        <v>113.52701070000001</v>
+        <v>130.86597219999999</v>
       </c>
       <c r="K18" s="0">
-        <v>5.8935939794890757e-05</v>
+        <v>5.3628834649543933e-05</v>
       </c>
       <c r="L18" s="0">
-        <v>3.505735032845712e-07</v>
+        <v>-5.0041677592651383e-08</v>
       </c>
       <c r="M18" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="0">
-        <v>0</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
@@ -881,7 +881,7 @@
         <v>2.5</v>
       </c>
       <c r="E19" s="0">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F19" s="0">
         <v>100</v>
@@ -893,22 +893,22 @@
         <v>10</v>
       </c>
       <c r="I19" s="0">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="J19" s="0">
-        <v>91.0562714</v>
+        <v>101.75489810000001</v>
       </c>
       <c r="K19" s="0">
-        <v>0.00027710452608475933</v>
+        <v>0.0079417695032171221</v>
       </c>
       <c r="L19" s="0">
-        <v>-2.5931324331350496e-05</v>
+        <v>8.4237720868004531e-05</v>
       </c>
       <c r="M19" s="0">
         <v>1</v>
       </c>
       <c r="N19" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20">
@@ -925,7 +925,7 @@
         <v>2.5</v>
       </c>
       <c r="E20" s="0">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="F20" s="0">
         <v>100</v>
@@ -937,22 +937,22 @@
         <v>10</v>
       </c>
       <c r="I20" s="0">
-        <v>270</v>
+        <v>497</v>
       </c>
       <c r="J20" s="0">
-        <v>229.43264070000001</v>
+        <v>341.550275</v>
       </c>
       <c r="K20" s="0">
-        <v>0.00079064481816271126</v>
+        <v>0.00043028847265680348</v>
       </c>
       <c r="L20" s="0">
-        <v>-3.2910294373719623e-05</v>
+        <v>-0.012764643082590781</v>
       </c>
       <c r="M20" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N20" s="0">
-        <v>173</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>